<commit_message>
Add some missing translations
</commit_message>
<xml_diff>
--- a/translations/census_household_translate_welsh.xlsx
+++ b/translations/census_household_translate_welsh.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1640" uniqueCount="1078">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1650" uniqueCount="1088">
   <si>
     <t>Context</t>
   </si>
@@ -3261,6 +3261,36 @@
   </si>
   <si>
     <t xml:space="preserve">Os ydych (oeddech) yn swyddog llywodraeth leol, ysgrifennwch swyddog llywodraeth leol, ysgrifennwch &lt;b&gt;llywodraeth leol&lt;/b&gt; a rhowch enw'r adran o fewn yr awdurdod lleol </t>
+  </si>
+  <si>
+    <t>Relationships</t>
+  </si>
+  <si>
+    <t>Household Member Details</t>
+  </si>
+  <si>
+    <t>Please specify other Black / African / Caribbean background</t>
+  </si>
+  <si>
+    <t>If you are (were) a local government officer, write &lt;b&gt;local government&lt;/b&gt; and give the name of the department within the local authority</t>
+  </si>
+  <si>
+    <t>Visitors</t>
+  </si>
+  <si>
+    <t>You have successfully completed the ‘Visitors’ section</t>
+  </si>
+  <si>
+    <t>Questionnaire Completed</t>
+  </si>
+  <si>
+    <t>Ymwelwyr</t>
+  </si>
+  <si>
+    <t>Rydych wedi cwblhau'r adran 'Ymwelwyr' yn llwyddiannus</t>
+  </si>
+  <si>
+    <t>Nodwch gefndir Du / Affricanaidd / Caribïaidd arall</t>
   </si>
 </sst>
 </file>
@@ -3614,10 +3644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C655"/>
+  <dimension ref="A1:C663"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A640" workbookViewId="0">
-      <selection activeCell="C652" sqref="C652"/>
+    <sheetView tabSelected="1" topLeftCell="A642" workbookViewId="0">
+      <selection activeCell="C663" sqref="C663"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3649,7 +3679,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -3671,7 +3701,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="105" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="75" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -3682,7 +3712,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -3757,7 +3787,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="105" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="75" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
@@ -3768,7 +3798,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
@@ -3832,7 +3862,7 @@
       </c>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
@@ -3843,7 +3873,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="60" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
@@ -3923,7 +3953,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>36</v>
       </c>
@@ -4114,7 +4144,7 @@
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C52" s="1"/>
     </row>
-    <row r="53" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>61</v>
       </c>
@@ -4139,7 +4169,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>64</v>
       </c>
@@ -4225,7 +4255,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>77</v>
       </c>
@@ -4374,7 +4404,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>97</v>
       </c>
@@ -4385,7 +4415,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>97</v>
       </c>
@@ -4396,7 +4426,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>97</v>
       </c>
@@ -4443,7 +4473,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>104</v>
       </c>
@@ -4454,7 +4484,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>104</v>
       </c>
@@ -4527,7 +4557,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>115</v>
       </c>
@@ -4538,7 +4568,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="330" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:3" ht="240" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>118</v>
       </c>
@@ -4660,7 +4690,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="75" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>131</v>
       </c>
@@ -4682,7 +4712,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>135</v>
       </c>
@@ -4718,7 +4748,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="120" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:3" ht="90" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>139</v>
       </c>
@@ -4892,7 +4922,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>154</v>
       </c>
@@ -4997,7 +5027,7 @@
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C144" s="1"/>
     </row>
-    <row r="145" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>156</v>
       </c>
@@ -5030,7 +5060,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="148" spans="1:3" ht="60" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>159</v>
       </c>
@@ -5052,7 +5082,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="150" spans="1:3" ht="75" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>164</v>
       </c>
@@ -5063,7 +5093,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="151" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>164</v>
       </c>
@@ -5074,7 +5104,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="152" spans="1:3" ht="90" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:3" ht="60" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
         <v>167</v>
       </c>
@@ -5096,7 +5126,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="154" spans="1:3" ht="60" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>167</v>
       </c>
@@ -5107,7 +5137,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="155" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>167</v>
       </c>
@@ -5129,7 +5159,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="157" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>167</v>
       </c>
@@ -5140,7 +5170,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="158" spans="1:3" ht="60" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>167</v>
       </c>
@@ -5162,7 +5192,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="160" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>167</v>
       </c>
@@ -5228,7 +5258,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="166" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>167</v>
       </c>
@@ -5259,7 +5289,7 @@
       </c>
       <c r="C169" s="1"/>
     </row>
-    <row r="170" spans="1:3" ht="75" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
         <v>185</v>
       </c>
@@ -5270,7 +5300,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="171" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
         <v>185</v>
       </c>
@@ -5281,7 +5311,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="172" spans="1:3" ht="60" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
         <v>186</v>
       </c>
@@ -5292,7 +5322,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="173" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
         <v>186</v>
       </c>
@@ -5303,7 +5333,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="174" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
         <v>186</v>
       </c>
@@ -5325,7 +5355,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="176" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
         <v>186</v>
       </c>
@@ -5336,7 +5366,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="177" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
         <v>186</v>
       </c>
@@ -5347,7 +5377,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="178" spans="1:3" ht="60" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
         <v>186</v>
       </c>
@@ -5358,7 +5388,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="179" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
         <v>186</v>
       </c>
@@ -5369,7 +5399,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="180" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
         <v>186</v>
       </c>
@@ -5435,7 +5465,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="186" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
         <v>186</v>
       </c>
@@ -5488,7 +5518,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="192" spans="1:3" ht="105" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:3" ht="75" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
         <v>197</v>
       </c>
@@ -5499,7 +5529,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="193" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
         <v>199</v>
       </c>
@@ -5546,7 +5576,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="198" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
         <v>204</v>
       </c>
@@ -5557,7 +5587,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="199" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
         <v>204</v>
       </c>
@@ -5579,7 +5609,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="201" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
         <v>204</v>
       </c>
@@ -5665,7 +5695,7 @@
       </c>
       <c r="C209" s="1"/>
     </row>
-    <row r="210" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
         <v>220</v>
       </c>
@@ -5676,7 +5706,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="211" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
         <v>220</v>
       </c>
@@ -5687,7 +5717,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="212" spans="1:3" ht="60" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
         <v>223</v>
       </c>
@@ -5709,7 +5739,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="214" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
         <v>225</v>
       </c>
@@ -5731,7 +5761,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="216" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
         <v>225</v>
       </c>
@@ -5875,7 +5905,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="231" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A231" s="1" t="s">
         <v>243</v>
       </c>
@@ -5886,7 +5916,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="232" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A232" s="1" t="s">
         <v>243</v>
       </c>
@@ -5897,7 +5927,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="233" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A233" s="1" t="s">
         <v>243</v>
       </c>
@@ -5944,7 +5974,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="238" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A238" s="1" t="s">
         <v>250</v>
       </c>
@@ -5955,7 +5985,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="239" spans="1:3" ht="60" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A239" s="1" t="s">
         <v>250</v>
       </c>
@@ -5966,7 +5996,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="240" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A240" s="1" t="s">
         <v>250</v>
       </c>
@@ -6010,7 +6040,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="244" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A244" s="1" t="s">
         <v>257</v>
       </c>
@@ -6021,7 +6051,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="245" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A245" s="1" t="s">
         <v>260</v>
       </c>
@@ -6136,7 +6166,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="259" spans="1:3" ht="105" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:3" ht="75" x14ac:dyDescent="0.2">
       <c r="A259" s="1" t="s">
         <v>275</v>
       </c>
@@ -6189,7 +6219,7 @@
       </c>
       <c r="C264" s="1"/>
     </row>
-    <row r="265" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A265" s="1" t="s">
         <v>281</v>
       </c>
@@ -6286,7 +6316,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="275" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A275" s="1" t="s">
         <v>291</v>
       </c>
@@ -6319,7 +6349,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="278" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A278" s="1" t="s">
         <v>291</v>
       </c>
@@ -6355,7 +6385,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="282" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A282" s="1" t="s">
         <v>298</v>
       </c>
@@ -6366,7 +6396,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="283" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A283" s="1" t="s">
         <v>300</v>
       </c>
@@ -6413,7 +6443,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="288" spans="1:3" ht="75" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A288" s="1" t="s">
         <v>306</v>
       </c>
@@ -6457,7 +6487,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="292" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A292" s="1" t="s">
         <v>313</v>
       </c>
@@ -6523,7 +6553,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="298" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A298" s="1" t="s">
         <v>317</v>
       </c>
@@ -6556,7 +6586,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="301" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A301" s="1" t="s">
         <v>317</v>
       </c>
@@ -6576,7 +6606,7 @@
       </c>
       <c r="C303" s="1"/>
     </row>
-    <row r="304" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A304" s="1" t="s">
         <v>325</v>
       </c>
@@ -6642,7 +6672,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="310" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A310" s="1" t="s">
         <v>327</v>
       </c>
@@ -6675,7 +6705,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="313" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A313" s="1" t="s">
         <v>327</v>
       </c>
@@ -6706,7 +6736,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="317" spans="1:3" ht="105" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:3" ht="75" x14ac:dyDescent="0.2">
       <c r="A317" s="1" t="s">
         <v>331</v>
       </c>
@@ -6792,7 +6822,7 @@
       </c>
       <c r="C325" s="1"/>
     </row>
-    <row r="326" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A326" s="1" t="s">
         <v>341</v>
       </c>
@@ -6836,7 +6866,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="330" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A330" s="1" t="s">
         <v>345</v>
       </c>
@@ -6847,7 +6877,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="331" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A331" s="1" t="s">
         <v>345</v>
       </c>
@@ -6880,7 +6910,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="334" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A334" s="1" t="s">
         <v>345</v>
       </c>
@@ -6933,7 +6963,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="340" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A340" s="1" t="s">
         <v>358</v>
       </c>
@@ -6955,7 +6985,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="342" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A342" s="1" t="s">
         <v>358</v>
       </c>
@@ -7019,7 +7049,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="349" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A349" s="1" t="s">
         <v>368</v>
       </c>
@@ -7030,7 +7060,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="350" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A350" s="1" t="s">
         <v>368</v>
       </c>
@@ -7061,7 +7091,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="354" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A354" s="1" t="s">
         <v>375</v>
       </c>
@@ -7114,7 +7144,7 @@
       </c>
       <c r="C359" s="1"/>
     </row>
-    <row r="360" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A360" s="1" t="s">
         <v>382</v>
       </c>
@@ -7346,7 +7376,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="383" spans="1:3" ht="60" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A383" s="1" t="s">
         <v>404</v>
       </c>
@@ -7368,7 +7398,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="385" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A385" s="1" t="s">
         <v>404</v>
       </c>
@@ -7421,7 +7451,7 @@
       </c>
       <c r="C390" s="1"/>
     </row>
-    <row r="391" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A391" s="1" t="s">
         <v>411</v>
       </c>
@@ -7463,7 +7493,7 @@
       </c>
       <c r="C395" s="1"/>
     </row>
-    <row r="396" spans="1:3" ht="75" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:3" ht="60" x14ac:dyDescent="0.2">
       <c r="A396" s="1" t="s">
         <v>415</v>
       </c>
@@ -7474,7 +7504,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="397" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A397" s="1" t="s">
         <v>417</v>
       </c>
@@ -7485,7 +7515,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="398" spans="1:3" ht="75" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:3" ht="60" x14ac:dyDescent="0.2">
       <c r="A398" s="1" t="s">
         <v>419</v>
       </c>
@@ -7516,7 +7546,7 @@
       </c>
       <c r="C401" s="1"/>
     </row>
-    <row r="402" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A402" s="1" t="s">
         <v>424</v>
       </c>
@@ -7600,7 +7630,7 @@
       </c>
       <c r="C411" s="1"/>
     </row>
-    <row r="412" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A412" s="1" t="s">
         <v>435</v>
       </c>
@@ -7653,7 +7683,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="418" spans="1:3" ht="255" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:3" ht="180" x14ac:dyDescent="0.2">
       <c r="A418" s="1" t="s">
         <v>441</v>
       </c>
@@ -7711,7 +7741,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="424" spans="1:3" ht="60" x14ac:dyDescent="0.2">
+    <row r="424" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A424" s="1" t="s">
         <v>445</v>
       </c>
@@ -7722,7 +7752,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="425" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="425" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A425" s="1" t="s">
         <v>445</v>
       </c>
@@ -7733,7 +7763,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="426" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="426" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A426" s="1" t="s">
         <v>445</v>
       </c>
@@ -7744,7 +7774,7 @@
         <v>934</v>
       </c>
     </row>
-    <row r="427" spans="1:3" ht="60" x14ac:dyDescent="0.2">
+    <row r="427" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A427" s="1" t="s">
         <v>445</v>
       </c>
@@ -7755,7 +7785,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="428" spans="1:3" ht="60" x14ac:dyDescent="0.2">
+    <row r="428" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A428" s="1" t="s">
         <v>445</v>
       </c>
@@ -7931,7 +7961,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="444" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="444" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A444" s="1" t="s">
         <v>455</v>
       </c>
@@ -7959,7 +7989,7 @@
     <row r="447" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C447" s="1"/>
     </row>
-    <row r="448" spans="1:3" ht="75" x14ac:dyDescent="0.2">
+    <row r="448" spans="1:3" ht="60" x14ac:dyDescent="0.2">
       <c r="A448" s="1" t="s">
         <v>472</v>
       </c>
@@ -7995,7 +8025,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="452" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="452" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A452" s="1" t="s">
         <v>475</v>
       </c>
@@ -8006,7 +8036,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="453" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="453" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A453" s="1" t="s">
         <v>475</v>
       </c>
@@ -8028,7 +8058,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="455" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="455" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A455" s="1" t="s">
         <v>475</v>
       </c>
@@ -8136,7 +8166,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="467" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="467" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A467" s="1" t="s">
         <v>485</v>
       </c>
@@ -8147,7 +8177,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="468" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="468" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A468" s="1" t="s">
         <v>485</v>
       </c>
@@ -8169,7 +8199,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="470" spans="1:3" ht="60" x14ac:dyDescent="0.2">
+    <row r="470" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A470" s="1" t="s">
         <v>485</v>
       </c>
@@ -8180,7 +8210,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="471" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="471" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A471" s="1" t="s">
         <v>485</v>
       </c>
@@ -8191,7 +8221,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="472" spans="1:3" ht="60" x14ac:dyDescent="0.2">
+    <row r="472" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A472" s="1" t="s">
         <v>492</v>
       </c>
@@ -8202,7 +8232,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="473" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="473" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A473" s="1" t="s">
         <v>492</v>
       </c>
@@ -8224,7 +8254,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="475" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="475" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A475" s="1" t="s">
         <v>495</v>
       </c>
@@ -8255,7 +8285,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="479" spans="1:3" ht="135" x14ac:dyDescent="0.2">
+    <row r="479" spans="1:3" ht="105" x14ac:dyDescent="0.2">
       <c r="A479" s="1" t="s">
         <v>500</v>
       </c>
@@ -8299,7 +8329,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="483" spans="1:3" ht="165" x14ac:dyDescent="0.2">
+    <row r="483" spans="1:3" ht="135" x14ac:dyDescent="0.2">
       <c r="A483" s="1" t="s">
         <v>505</v>
       </c>
@@ -8310,7 +8340,7 @@
         <v>969</v>
       </c>
     </row>
-    <row r="484" spans="1:3" ht="75" x14ac:dyDescent="0.2">
+    <row r="484" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A484" s="1" t="s">
         <v>507</v>
       </c>
@@ -8332,7 +8362,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="486" spans="1:3" ht="60" x14ac:dyDescent="0.2">
+    <row r="486" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A486" s="1" t="s">
         <v>507</v>
       </c>
@@ -8354,7 +8384,7 @@
         <v>973</v>
       </c>
     </row>
-    <row r="488" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="488" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A488" s="1" t="s">
         <v>507</v>
       </c>
@@ -8376,7 +8406,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="490" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="490" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A490" s="1" t="s">
         <v>507</v>
       </c>
@@ -8387,7 +8417,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="491" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="491" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A491" s="1" t="s">
         <v>507</v>
       </c>
@@ -8398,7 +8428,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="492" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="492" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A492" s="1" t="s">
         <v>507</v>
       </c>
@@ -8440,7 +8470,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="497" spans="1:3" ht="165" x14ac:dyDescent="0.2">
+    <row r="497" spans="1:3" ht="135" x14ac:dyDescent="0.2">
       <c r="A497" s="1" t="s">
         <v>520</v>
       </c>
@@ -8451,7 +8481,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="498" spans="1:3" ht="75" x14ac:dyDescent="0.2">
+    <row r="498" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A498" s="1" t="s">
         <v>522</v>
       </c>
@@ -8473,7 +8503,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="500" spans="1:3" ht="60" x14ac:dyDescent="0.2">
+    <row r="500" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A500" s="1" t="s">
         <v>522</v>
       </c>
@@ -8495,7 +8525,7 @@
         <v>973</v>
       </c>
     </row>
-    <row r="502" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="502" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A502" s="1" t="s">
         <v>522</v>
       </c>
@@ -8517,7 +8547,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="504" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="504" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A504" s="1" t="s">
         <v>522</v>
       </c>
@@ -8528,7 +8558,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="505" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="505" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A505" s="1" t="s">
         <v>522</v>
       </c>
@@ -8539,7 +8569,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="506" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="506" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A506" s="1" t="s">
         <v>522</v>
       </c>
@@ -8634,7 +8664,7 @@
       </c>
       <c r="C516" s="1"/>
     </row>
-    <row r="517" spans="1:3" ht="60" x14ac:dyDescent="0.2">
+    <row r="517" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A517" s="1" t="s">
         <v>533</v>
       </c>
@@ -8678,7 +8708,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="521" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="521" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A521" s="1" t="s">
         <v>537</v>
       </c>
@@ -8689,7 +8719,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="522" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="522" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A522" s="1" t="s">
         <v>537</v>
       </c>
@@ -8711,7 +8741,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="524" spans="1:3" ht="75" x14ac:dyDescent="0.2">
+    <row r="524" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A524" s="1" t="s">
         <v>537</v>
       </c>
@@ -8722,7 +8752,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="525" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="525" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A525" s="1" t="s">
         <v>537</v>
       </c>
@@ -8753,7 +8783,7 @@
       </c>
       <c r="C528" s="1"/>
     </row>
-    <row r="529" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="529" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A529" s="1" t="s">
         <v>546</v>
       </c>
@@ -8786,7 +8816,7 @@
         <v>1077</v>
       </c>
     </row>
-    <row r="532" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="532" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A532" s="1" t="s">
         <v>550</v>
       </c>
@@ -8797,7 +8827,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="533" spans="1:3" ht="180" x14ac:dyDescent="0.2">
+    <row r="533" spans="1:3" ht="135" x14ac:dyDescent="0.2">
       <c r="A533" s="1" t="s">
         <v>552</v>
       </c>
@@ -8855,7 +8885,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="539" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="539" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A539" s="1" t="s">
         <v>556</v>
       </c>
@@ -8866,7 +8896,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="540" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="540" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A540" s="1" t="s">
         <v>556</v>
       </c>
@@ -8888,7 +8918,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="542" spans="1:3" ht="60" x14ac:dyDescent="0.2">
+    <row r="542" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A542" s="1" t="s">
         <v>556</v>
       </c>
@@ -8899,7 +8929,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="543" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="543" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A543" s="1" t="s">
         <v>556</v>
       </c>
@@ -8910,7 +8940,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="544" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="544" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A544" s="1" t="s">
         <v>560</v>
       </c>
@@ -8932,7 +8962,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="546" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="546" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A546" s="1" t="s">
         <v>563</v>
       </c>
@@ -8943,7 +8973,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="547" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="547" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A547" s="1" t="s">
         <v>563</v>
       </c>
@@ -8974,7 +9004,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="551" spans="1:3" ht="75" x14ac:dyDescent="0.2">
+    <row r="551" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A551" s="1" t="s">
         <v>569</v>
       </c>
@@ -9354,7 +9384,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="591" spans="1:3" ht="90" x14ac:dyDescent="0.2">
+    <row r="591" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A591" s="1" t="s">
         <v>604</v>
       </c>
@@ -9398,7 +9428,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="595" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="595" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A595" s="1" t="s">
         <v>607</v>
       </c>
@@ -9451,7 +9481,7 @@
       </c>
       <c r="C600" s="1"/>
     </row>
-    <row r="601" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="601" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A601" s="1" t="s">
         <v>615</v>
       </c>
@@ -9462,7 +9492,7 @@
         <v>1031</v>
       </c>
     </row>
-    <row r="602" spans="1:3" ht="60" x14ac:dyDescent="0.2">
+    <row r="602" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A602" s="1" t="s">
         <v>617</v>
       </c>
@@ -9473,7 +9503,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="603" spans="1:3" ht="60" x14ac:dyDescent="0.2">
+    <row r="603" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A603" s="1" t="s">
         <v>617</v>
       </c>
@@ -9537,7 +9567,7 @@
       </c>
       <c r="C609" s="1"/>
     </row>
-    <row r="610" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="610" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A610" s="1" t="s">
         <v>625</v>
       </c>
@@ -9548,7 +9578,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="611" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="611" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A611" s="1" t="s">
         <v>627</v>
       </c>
@@ -9559,7 +9589,7 @@
         <v>1038</v>
       </c>
     </row>
-    <row r="612" spans="1:3" ht="135" x14ac:dyDescent="0.2">
+    <row r="612" spans="1:3" ht="120" x14ac:dyDescent="0.2">
       <c r="A612" s="1" t="s">
         <v>629</v>
       </c>
@@ -9601,7 +9631,7 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="617" spans="1:3" ht="105" x14ac:dyDescent="0.2">
+    <row r="617" spans="1:3" ht="75" x14ac:dyDescent="0.2">
       <c r="A617" s="1" t="s">
         <v>636</v>
       </c>
@@ -9665,7 +9695,7 @@
       </c>
       <c r="C623" s="1"/>
     </row>
-    <row r="624" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="624" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A624" s="1" t="s">
         <v>643</v>
       </c>
@@ -9676,7 +9706,7 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="625" spans="1:3" ht="105" x14ac:dyDescent="0.2">
+    <row r="625" spans="1:3" ht="75" x14ac:dyDescent="0.2">
       <c r="A625" s="1" t="s">
         <v>645</v>
       </c>
@@ -9762,7 +9792,7 @@
       </c>
       <c r="C633" s="1"/>
     </row>
-    <row r="634" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="634" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A634" s="1" t="s">
         <v>654</v>
       </c>
@@ -9773,7 +9803,7 @@
         <v>1053</v>
       </c>
     </row>
-    <row r="635" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="635" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A635" s="1" t="s">
         <v>656</v>
       </c>
@@ -9815,7 +9845,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="640" spans="1:3" ht="120" x14ac:dyDescent="0.2">
+    <row r="640" spans="1:3" ht="75" x14ac:dyDescent="0.2">
       <c r="A640" s="1" t="s">
         <v>662</v>
       </c>
@@ -9848,7 +9878,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="643" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="643" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A643" s="1" t="s">
         <v>664</v>
       </c>
@@ -9879,7 +9909,7 @@
       </c>
       <c r="C646" s="1"/>
     </row>
-    <row r="647" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="647" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A647" s="1" t="s">
         <v>669</v>
       </c>
@@ -9890,7 +9920,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="648" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="648" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A648" s="1" t="s">
         <v>671</v>
       </c>
@@ -9934,7 +9964,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="652" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="652" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A652" s="1" t="s">
         <v>671</v>
       </c>
@@ -9976,6 +10006,52 @@
       </c>
       <c r="C655" s="2" t="s">
         <v>1067</v>
+      </c>
+    </row>
+    <row r="657" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B657" s="1" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="658" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B658" s="1" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C658" s="2"/>
+    </row>
+    <row r="659" spans="2:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="B659" s="1" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C659" s="2" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="660" spans="2:3" ht="45" x14ac:dyDescent="0.2">
+      <c r="B660" s="1" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C660" s="1"/>
+    </row>
+    <row r="661" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B661" s="1" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C661" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="662" spans="2:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="B662" s="1" t="s">
+        <v>1083</v>
+      </c>
+      <c r="C662" s="2" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="663" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B663" s="1" t="s">
+        <v>1084</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add translation to spreadsheet
</commit_message>
<xml_diff>
--- a/translations/census_household_translate_welsh.xlsx
+++ b/translations/census_household_translate_welsh.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1650" uniqueCount="1088">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1651" uniqueCount="1089">
   <si>
     <t>Context</t>
   </si>
@@ -3291,6 +3291,9 @@
   </si>
   <si>
     <t>Nodwch gefndir Du / Affricanaidd / Caribïaidd arall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Os ydych (oeddech) yn swyddog llywodraeth leol, ysgrifennwch &lt;b&gt;llywodraeth leol&lt;/b&gt; a rhowch enw'r adran o fewn yr awdurdod lleol </t>
   </si>
 </sst>
 </file>
@@ -3646,8 +3649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C663"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A642" workbookViewId="0">
-      <selection activeCell="C663" sqref="C663"/>
+    <sheetView tabSelected="1" topLeftCell="A649" workbookViewId="0">
+      <selection activeCell="C660" sqref="C660"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10031,7 +10034,9 @@
       <c r="B660" s="1" t="s">
         <v>1081</v>
       </c>
-      <c r="C660" s="1"/>
+      <c r="C660" s="2" t="s">
+        <v>1088</v>
+      </c>
     </row>
     <row r="661" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B661" s="1" t="s">

</xml_diff>

<commit_message>
Fix non-translated 'Include' text
</commit_message>
<xml_diff>
--- a/translations/census_household_translate_welsh.xlsx
+++ b/translations/census_household_translate_welsh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25320" windowHeight="14440"/>
+    <workbookView xWindow="-1860" yWindow="460" windowWidth="25320" windowHeight="14440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -3047,9 +3047,6 @@
     <t xml:space="preserve">Nid oes neb yn byw yma fel eu cartref parhaol </t>
   </si>
   <si>
-    <t>&lt;strong&gt;Include&lt;/strong&gt; Problemau sy'n gysylltiedig â henaint</t>
-  </si>
-  <si>
     <t>A oes gennych broblem iechyd neu anabledd sydd wedi para neu sy’n debygol o bara am o leiaf 12 mis, ac sy’n cyfyngu ar eich gallu i wneud gweithgareddau arferol?</t>
   </si>
   <si>
@@ -3294,6 +3291,9 @@
   </si>
   <si>
     <t xml:space="preserve">Os ydych (oeddech) yn swyddog llywodraeth leol, ysgrifennwch &lt;b&gt;llywodraeth leol&lt;/b&gt; a rhowch enw'r adran o fewn yr awdurdod lleol </t>
+  </si>
+  <si>
+    <t>&lt;strong&gt;Dylech gynnwys&lt;/strong&gt; Problemau sy'n gysylltiedig â henaint</t>
   </si>
 </sst>
 </file>
@@ -3649,8 +3649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C663"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A649" workbookViewId="0">
-      <selection activeCell="C660" sqref="C660"/>
+    <sheetView tabSelected="1" topLeftCell="A441" workbookViewId="0">
+      <selection activeCell="B451" sqref="B451"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5894,7 +5894,7 @@
         <v>242</v>
       </c>
       <c r="C229" s="2" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.2">
@@ -6509,7 +6509,7 @@
         <v>316</v>
       </c>
       <c r="C293" s="2" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.2">
@@ -6628,7 +6628,7 @@
         <v>316</v>
       </c>
       <c r="C305" s="2" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.2">
@@ -6844,7 +6844,7 @@
         <v>344</v>
       </c>
       <c r="C327" s="2" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="328" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -7027,7 +7027,7 @@
         <v>365</v>
       </c>
       <c r="C346" s="2" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.2">
@@ -7221,7 +7221,7 @@
         <v>390</v>
       </c>
       <c r="C366" s="2" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="367" spans="1:3" x14ac:dyDescent="0.2">
@@ -7610,7 +7610,7 @@
         <v>431</v>
       </c>
       <c r="C408" s="2" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="409" spans="1:3" x14ac:dyDescent="0.2">
@@ -8166,7 +8166,7 @@
         <v>486</v>
       </c>
       <c r="C466" s="2" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="467" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -8199,7 +8199,7 @@
         <v>489</v>
       </c>
       <c r="C469" s="2" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="470" spans="1:3" ht="45" x14ac:dyDescent="0.2">
@@ -8816,7 +8816,7 @@
         <v>549</v>
       </c>
       <c r="C531" s="2" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="532" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -8885,7 +8885,7 @@
         <v>486</v>
       </c>
       <c r="C538" s="2" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="539" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -8918,7 +8918,7 @@
         <v>489</v>
       </c>
       <c r="C541" s="2" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="542" spans="1:3" ht="45" x14ac:dyDescent="0.2">
@@ -9004,7 +9004,7 @@
         <v>568</v>
       </c>
       <c r="C550" s="2" t="s">
-        <v>1006</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="551" spans="1:3" ht="45" x14ac:dyDescent="0.2">
@@ -9015,7 +9015,7 @@
         <v>570</v>
       </c>
       <c r="C551" s="2" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="552" spans="1:3" x14ac:dyDescent="0.2">
@@ -9026,7 +9026,7 @@
         <v>572</v>
       </c>
       <c r="C552" s="2" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="553" spans="1:3" x14ac:dyDescent="0.2">
@@ -9037,7 +9037,7 @@
         <v>573</v>
       </c>
       <c r="C553" s="2" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="554" spans="1:3" x14ac:dyDescent="0.2">
@@ -9068,7 +9068,7 @@
         <v>576</v>
       </c>
       <c r="C557" s="2" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="558" spans="1:3" x14ac:dyDescent="0.2">
@@ -9079,7 +9079,7 @@
         <v>578</v>
       </c>
       <c r="C558" s="2" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="559" spans="1:3" x14ac:dyDescent="0.2">
@@ -9090,7 +9090,7 @@
         <v>579</v>
       </c>
       <c r="C559" s="2" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="560" spans="1:3" x14ac:dyDescent="0.2">
@@ -9121,7 +9121,7 @@
         <v>582</v>
       </c>
       <c r="C563" s="2" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="564" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -9143,7 +9143,7 @@
         <v>585</v>
       </c>
       <c r="C565" s="2" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="566" spans="1:3" x14ac:dyDescent="0.2">
@@ -9154,7 +9154,7 @@
         <v>587</v>
       </c>
       <c r="C566" s="2" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="567" spans="1:3" x14ac:dyDescent="0.2">
@@ -9165,7 +9165,7 @@
         <v>588</v>
       </c>
       <c r="C567" s="2" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="568" spans="1:3" x14ac:dyDescent="0.2">
@@ -9176,7 +9176,7 @@
         <v>589</v>
       </c>
       <c r="C568" s="2" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="569" spans="1:3" x14ac:dyDescent="0.2">
@@ -9187,7 +9187,7 @@
         <v>590</v>
       </c>
       <c r="C569" s="2" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="570" spans="1:3" x14ac:dyDescent="0.2">
@@ -9198,7 +9198,7 @@
         <v>591</v>
       </c>
       <c r="C570" s="2" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="571" spans="1:3" x14ac:dyDescent="0.2">
@@ -9209,7 +9209,7 @@
         <v>592</v>
       </c>
       <c r="C571" s="2" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="572" spans="1:3" x14ac:dyDescent="0.2">
@@ -9220,7 +9220,7 @@
         <v>593</v>
       </c>
       <c r="C572" s="2" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="573" spans="1:3" x14ac:dyDescent="0.2">
@@ -9240,7 +9240,7 @@
         <v>585</v>
       </c>
       <c r="C575" s="2" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="576" spans="1:3" x14ac:dyDescent="0.2">
@@ -9251,7 +9251,7 @@
         <v>588</v>
       </c>
       <c r="C576" s="2" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="577" spans="1:3" x14ac:dyDescent="0.2">
@@ -9262,7 +9262,7 @@
         <v>587</v>
       </c>
       <c r="C577" s="2" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="578" spans="1:3" x14ac:dyDescent="0.2">
@@ -9273,7 +9273,7 @@
         <v>589</v>
       </c>
       <c r="C578" s="2" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="579" spans="1:3" x14ac:dyDescent="0.2">
@@ -9284,7 +9284,7 @@
         <v>590</v>
       </c>
       <c r="C579" s="2" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="580" spans="1:3" x14ac:dyDescent="0.2">
@@ -9295,7 +9295,7 @@
         <v>591</v>
       </c>
       <c r="C580" s="2" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="581" spans="1:3" x14ac:dyDescent="0.2">
@@ -9306,7 +9306,7 @@
         <v>592</v>
       </c>
       <c r="C581" s="2" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="582" spans="1:3" x14ac:dyDescent="0.2">
@@ -9317,7 +9317,7 @@
         <v>593</v>
       </c>
       <c r="C582" s="2" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="583" spans="1:3" x14ac:dyDescent="0.2">
@@ -9337,7 +9337,7 @@
         <v>599</v>
       </c>
       <c r="C585" s="2" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="586" spans="1:3" x14ac:dyDescent="0.2">
@@ -9395,7 +9395,7 @@
         <v>605</v>
       </c>
       <c r="C591" s="2" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="592" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -9406,7 +9406,7 @@
         <v>606</v>
       </c>
       <c r="C592" s="2" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="593" spans="1:3" x14ac:dyDescent="0.2">
@@ -9417,7 +9417,7 @@
         <v>608</v>
       </c>
       <c r="C593" s="2" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="594" spans="1:3" x14ac:dyDescent="0.2">
@@ -9428,7 +9428,7 @@
         <v>609</v>
       </c>
       <c r="C594" s="2" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="595" spans="1:3" x14ac:dyDescent="0.2">
@@ -9439,7 +9439,7 @@
         <v>610</v>
       </c>
       <c r="C595" s="2" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="596" spans="1:3" x14ac:dyDescent="0.2">
@@ -9450,7 +9450,7 @@
         <v>611</v>
       </c>
       <c r="C596" s="2" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="597" spans="1:3" x14ac:dyDescent="0.2">
@@ -9461,7 +9461,7 @@
         <v>612</v>
       </c>
       <c r="C597" s="2" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="598" spans="1:3" x14ac:dyDescent="0.2">
@@ -9472,7 +9472,7 @@
         <v>613</v>
       </c>
       <c r="C598" s="2" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="599" spans="1:3" x14ac:dyDescent="0.2">
@@ -9492,7 +9492,7 @@
         <v>616</v>
       </c>
       <c r="C601" s="2" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="602" spans="1:3" ht="45" x14ac:dyDescent="0.2">
@@ -9503,7 +9503,7 @@
         <v>618</v>
       </c>
       <c r="C602" s="2" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="603" spans="1:3" ht="45" x14ac:dyDescent="0.2">
@@ -9514,7 +9514,7 @@
         <v>619</v>
       </c>
       <c r="C603" s="2" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="604" spans="1:3" x14ac:dyDescent="0.2">
@@ -9536,7 +9536,7 @@
         <v>621</v>
       </c>
       <c r="C605" s="2" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="606" spans="1:3" x14ac:dyDescent="0.2">
@@ -9547,7 +9547,7 @@
         <v>622</v>
       </c>
       <c r="C606" s="2" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="607" spans="1:3" x14ac:dyDescent="0.2">
@@ -9558,7 +9558,7 @@
         <v>623</v>
       </c>
       <c r="C607" s="2" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="608" spans="1:3" x14ac:dyDescent="0.2">
@@ -9578,7 +9578,7 @@
         <v>626</v>
       </c>
       <c r="C610" s="2" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="611" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -9589,7 +9589,7 @@
         <v>628</v>
       </c>
       <c r="C611" s="2" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="612" spans="1:3" ht="120" x14ac:dyDescent="0.2">
@@ -9600,7 +9600,7 @@
         <v>630</v>
       </c>
       <c r="C612" s="2" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="613" spans="1:3" x14ac:dyDescent="0.2">
@@ -9611,7 +9611,7 @@
         <v>632</v>
       </c>
       <c r="C613" s="2" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="614" spans="1:3" x14ac:dyDescent="0.2">
@@ -9631,7 +9631,7 @@
         <v>635</v>
       </c>
       <c r="C616" s="2" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="617" spans="1:3" ht="75" x14ac:dyDescent="0.2">
@@ -9653,7 +9653,7 @@
         <v>638</v>
       </c>
       <c r="C618" s="2" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="619" spans="1:3" x14ac:dyDescent="0.2">
@@ -9664,7 +9664,7 @@
         <v>639</v>
       </c>
       <c r="C619" s="2" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="620" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -9675,7 +9675,7 @@
         <v>640</v>
       </c>
       <c r="C620" s="2" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="621" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -9686,7 +9686,7 @@
         <v>641</v>
       </c>
       <c r="C621" s="2" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="622" spans="1:3" x14ac:dyDescent="0.2">
@@ -9706,7 +9706,7 @@
         <v>644</v>
       </c>
       <c r="C624" s="2" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="625" spans="1:3" ht="75" x14ac:dyDescent="0.2">
@@ -9728,7 +9728,7 @@
         <v>647</v>
       </c>
       <c r="C626" s="2" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="627" spans="1:3" x14ac:dyDescent="0.2">
@@ -9739,7 +9739,7 @@
         <v>648</v>
       </c>
       <c r="C627" s="2" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="628" spans="1:3" x14ac:dyDescent="0.2">
@@ -9750,7 +9750,7 @@
         <v>649</v>
       </c>
       <c r="C628" s="2" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="629" spans="1:3" x14ac:dyDescent="0.2">
@@ -9761,7 +9761,7 @@
         <v>650</v>
       </c>
       <c r="C629" s="2" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="630" spans="1:3" x14ac:dyDescent="0.2">
@@ -9772,7 +9772,7 @@
         <v>651</v>
       </c>
       <c r="C630" s="2" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="631" spans="1:3" x14ac:dyDescent="0.2">
@@ -9783,7 +9783,7 @@
         <v>652</v>
       </c>
       <c r="C631" s="2" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="632" spans="1:3" x14ac:dyDescent="0.2">
@@ -9803,7 +9803,7 @@
         <v>655</v>
       </c>
       <c r="C634" s="2" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="635" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -9814,7 +9814,7 @@
         <v>657</v>
       </c>
       <c r="C635" s="2" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="636" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -9845,7 +9845,7 @@
         <v>661</v>
       </c>
       <c r="C639" s="2" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="640" spans="1:3" ht="75" x14ac:dyDescent="0.2">
@@ -9856,7 +9856,7 @@
         <v>663</v>
       </c>
       <c r="C640" s="2" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="641" spans="1:3" x14ac:dyDescent="0.2">
@@ -9878,7 +9878,7 @@
         <v>665</v>
       </c>
       <c r="C642" s="2" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="643" spans="1:3" x14ac:dyDescent="0.2">
@@ -9889,7 +9889,7 @@
         <v>666</v>
       </c>
       <c r="C643" s="2" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="644" spans="1:3" x14ac:dyDescent="0.2">
@@ -9900,7 +9900,7 @@
         <v>667</v>
       </c>
       <c r="C644" s="2" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="645" spans="1:3" x14ac:dyDescent="0.2">
@@ -9920,7 +9920,7 @@
         <v>670</v>
       </c>
       <c r="C647" s="2" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="648" spans="1:3" x14ac:dyDescent="0.2">
@@ -9931,7 +9931,7 @@
         <v>672</v>
       </c>
       <c r="C648" s="2" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="649" spans="1:3" x14ac:dyDescent="0.2">
@@ -9942,7 +9942,7 @@
         <v>673</v>
       </c>
       <c r="C649" s="2" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="650" spans="1:3" x14ac:dyDescent="0.2">
@@ -9953,7 +9953,7 @@
         <v>674</v>
       </c>
       <c r="C650" s="2" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="651" spans="1:3" x14ac:dyDescent="0.2">
@@ -9964,7 +9964,7 @@
         <v>675</v>
       </c>
       <c r="C651" s="2" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="652" spans="1:3" x14ac:dyDescent="0.2">
@@ -9975,7 +9975,7 @@
         <v>676</v>
       </c>
       <c r="C652" s="2" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="653" spans="1:3" x14ac:dyDescent="0.2">
@@ -9986,7 +9986,7 @@
         <v>677</v>
       </c>
       <c r="C653" s="2" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="654" spans="1:3" x14ac:dyDescent="0.2">
@@ -10008,55 +10008,55 @@
         <v>678</v>
       </c>
       <c r="C655" s="2" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="657" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B657" s="1" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="658" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B658" s="1" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="C658" s="2"/>
     </row>
     <row r="659" spans="2:3" ht="30" x14ac:dyDescent="0.2">
       <c r="B659" s="1" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="C659" s="2" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="660" spans="2:3" ht="45" x14ac:dyDescent="0.2">
       <c r="B660" s="1" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="C660" s="2" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="661" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B661" s="1" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="C661" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="662" spans="2:3" ht="30" x14ac:dyDescent="0.2">
       <c r="B662" s="1" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="C662" s="2" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="663" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B663" s="1" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
   </sheetData>

</xml_diff>